<commit_message>
updated api endpoint + DB structure (added user + session tables)
</commit_message>
<xml_diff>
--- a/webapi/setup/API.xlsx
+++ b/webapi/setup/API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Mobile\iOS\home-hunt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Mobile\iOS\home-hunt\webapi\setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="23">
   <si>
     <t>Agents</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>/login</t>
+  </si>
+  <si>
+    <t>/register</t>
+  </si>
+  <si>
+    <t>/logout</t>
   </si>
 </sst>
 </file>
@@ -358,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -373,6 +382,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -391,11 +405,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,16 +699,16 @@
     <col min="5" max="5" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
@@ -712,321 +722,397 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="4" t="s">
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="14"/>
+      <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="5" t="s">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="17" t="s">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="2" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E25" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="7" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="7"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="8" t="s">
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="17" t="s">
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="2" t="s">
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
+      <c r="B33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="22" t="s">
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D34" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="22"/>
+      <c r="E34" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added base structure + login, logout logic
</commit_message>
<xml_diff>
--- a/webapi/setup/API.xlsx
+++ b/webapi/setup/API.xlsx
@@ -127,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +140,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -367,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -387,6 +393,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -405,7 +412,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +698,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,12 +710,12 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -723,7 +732,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -753,7 +762,7 @@
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="24" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -768,20 +777,20 @@
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -871,12 +880,12 @@
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
@@ -967,12 +976,12 @@
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
@@ -1069,12 +1078,12 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>

</xml_diff>

<commit_message>
update db script + postman collection
</commit_message>
<xml_diff>
--- a/webapi/setup/API.xlsx
+++ b/webapi/setup/API.xlsx
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1014,7 +1014,7 @@
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B27" s="4" t="s">
@@ -1029,7 +1029,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1044,7 +1044,7 @@
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="4" t="s">
@@ -1059,7 +1059,7 @@
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -1101,7 +1101,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B34" s="15" t="s">

</xml_diff>